<commit_message>
correccion lector datos excel
</commit_message>
<xml_diff>
--- a/prueba5_excel.xlsx
+++ b/prueba5_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enkro\Automatizacion_DiagramasDeFlujo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enkross.sharepoint.com/sites/ENKROSSCloud/Proyectos/P00106-ENKROSS (INTERNO 2024)/03_Ingeniería/Desarrollo unifilares/P00106-ENKROSS_PRUEBA3_AUTOMATIZACION/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1737B8-D03B-463F-9A03-ED9ED9C11095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{8A1737B8-D03B-463F-9A03-ED9ED9C11095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB0FE3C0-F608-4AD3-BA78-828A5E27177C}"/>
   <bookViews>
-    <workbookView xWindow="2004" yWindow="2100" windowWidth="28668" windowHeight="12168" xr2:uid="{A51B9455-0DA1-4262-9C8D-5E63C3C80935}"/>
+    <workbookView minimized="1" xWindow="372" yWindow="1992" windowWidth="28668" windowHeight="14568" xr2:uid="{A51B9455-0DA1-4262-9C8D-5E63C3C80935}"/>
   </bookViews>
   <sheets>
     <sheet name="diagrama1" sheetId="1" r:id="rId1"/>
@@ -180,6 +180,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -502,7 +506,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,10 +534,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -882,9 +886,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845E6CD6-41F1-467B-BEAF-28FF031A1554}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845E6CD6-41F1-467B-BEAF-28FF031A1554}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4578e3cf-dc59-46b9-b473-9d64d86ba65a"/>
+    <ds:schemaRef ds:uri="565c94a9-9f9d-407f-a547-016888b2b680"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D297736C-B56D-4755-88CF-1B2FF5BC0647}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D297736C-B56D-4755-88CF-1B2FF5BC0647}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>